<commit_message>
new story link, corrected error demand reading
</commit_message>
<xml_diff>
--- a/Tests/Database input/ERROR_DEMAND.xlsx
+++ b/Tests/Database input/ERROR_DEMAND.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -556,7 +556,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -719,7 +719,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -752,7 +752,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -785,7 +785,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -818,7 +818,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -884,7 +884,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -917,7 +917,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -950,7 +950,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -983,7 +983,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1214,7 +1214,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1610,7 +1610,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -1808,7 +1808,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -1940,7 +1940,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -1973,7 +1973,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2105,7 +2105,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -2204,7 +2204,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2237,7 +2237,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G57" t="n">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -2402,7 +2402,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G60" t="n">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G61" t="n">
@@ -2468,7 +2468,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G63" t="n">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G64" t="n">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G65" t="n">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -2666,7 +2666,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -2699,7 +2699,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -2732,7 +2732,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G71" t="n">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G72" t="n">
@@ -2831,7 +2831,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -2864,7 +2864,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G79" t="n">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G80" t="n">
@@ -3095,7 +3095,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G81" t="n">
@@ -3128,7 +3128,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G82" t="n">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G83" t="n">
@@ -3194,7 +3194,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -3227,7 +3227,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G86" t="n">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G87" t="n">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G88" t="n">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G89" t="n">
@@ -3392,7 +3392,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G90" t="n">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G91" t="n">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G92" t="n">
@@ -3491,7 +3491,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G93" t="n">
@@ -3524,7 +3524,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -3557,7 +3557,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G95" t="n">
@@ -3590,7 +3590,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G97" t="n">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G99" t="n">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G100" t="n">
@@ -3755,7 +3755,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G101" t="n">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -3854,7 +3854,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G104" t="n">
@@ -3887,7 +3887,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -3920,7 +3920,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G106" t="n">
@@ -3953,7 +3953,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -3986,7 +3986,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G108" t="n">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G109" t="n">
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G110" t="n">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G112" t="n">
@@ -4151,7 +4151,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G113" t="n">
@@ -4184,7 +4184,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G114" t="n">
@@ -4217,7 +4217,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G115" t="n">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G116" t="n">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G117" t="n">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G118" t="n">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G119" t="n">
@@ -4382,7 +4382,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G120" t="n">
@@ -4415,7 +4415,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G121" t="n">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G122" t="n">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G123" t="n">
@@ -4514,7 +4514,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G124" t="n">
@@ -4547,7 +4547,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -4580,7 +4580,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G127" t="n">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G128" t="n">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G129" t="n">
@@ -4712,7 +4712,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G130" t="n">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G131" t="n">
@@ -4778,7 +4778,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G132" t="n">
@@ -4811,7 +4811,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G133" t="n">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G134" t="n">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G135" t="n">
@@ -4910,7 +4910,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -4976,7 +4976,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G138" t="n">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G139" t="n">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G140" t="n">
@@ -5075,7 +5075,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G141" t="n">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G142" t="n">
@@ -5141,7 +5141,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G143" t="n">
@@ -5174,7 +5174,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G144" t="n">
@@ -5207,7 +5207,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G145" t="n">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G146" t="n">
@@ -5269,7 +5269,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G147" t="n">
@@ -5300,7 +5300,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G148" t="n">
@@ -5331,7 +5331,7 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G149" t="n">
@@ -5362,7 +5362,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G150" t="n">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G151" t="n">
@@ -5424,7 +5424,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G152" t="n">
@@ -5455,7 +5455,7 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G153" t="n">
@@ -5486,7 +5486,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G154" t="n">
@@ -5517,7 +5517,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G155" t="n">
@@ -5548,7 +5548,7 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G156" t="n">
@@ -5579,7 +5579,7 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G157" t="n">
@@ -5610,7 +5610,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G158" t="n">
@@ -5641,7 +5641,7 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G159" t="n">
@@ -5672,7 +5672,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G160" t="n">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G161" t="n">
@@ -5734,7 +5734,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G162" t="n">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G163" t="n">
@@ -5796,7 +5796,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G164" t="n">
@@ -5827,7 +5827,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>2021-10-13</t>
+          <t>2021-10-28</t>
         </is>
       </c>
       <c r="G165" t="n">

</xml_diff>